<commit_message>
update full override model with UCRP return scenarios
</commit_message>
<xml_diff>
--- a/FullOverride/RunControl_fullOverride.xlsx
+++ b/FullOverride/RunControl_fullOverride.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>runname</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>RS1.Cap</t>
+  </si>
+  <si>
+    <t>internal</t>
+  </si>
+  <si>
+    <t>RS1.ADC</t>
   </si>
 </sst>
 </file>
@@ -603,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AB18"/>
+  <dimension ref="A4:AB19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1499,7 @@
         <v>1</v>
       </c>
       <c r="T18" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="U18" t="s">
         <v>43</v>
@@ -1502,7 +1508,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
       <c r="W18">
-        <f t="shared" ref="W18" si="2">0.0797</f>
+        <f t="shared" ref="W18:W19" si="2">0.0797</f>
         <v>7.9699999999999993E-2</v>
       </c>
       <c r="X18">
@@ -1521,10 +1527,97 @@
         <v>15</v>
       </c>
     </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2000</v>
+      </c>
+      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>16</v>
+      </c>
+      <c r="O19">
+        <v>20</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19" t="s">
+        <v>53</v>
+      </c>
+      <c r="U19" t="s">
+        <v>43</v>
+      </c>
+      <c r="V19">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="2"/>
+        <v>7.9699999999999993E-2</v>
+      </c>
+      <c r="X19">
+        <v>0.12</v>
+      </c>
+      <c r="Y19">
+        <v>20</v>
+      </c>
+      <c r="Z19">
+        <v>20</v>
+      </c>
+      <c r="AA19">
+        <v>30</v>
+      </c>
+      <c r="AB19">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C18">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C19">
       <formula1>"TRUE, FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T19">
+      <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1537,7 +1630,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated version of return scenarios in the full override model.
</commit_message>
<xml_diff>
--- a/FullOverride/RunControl_fullOverride.xlsx
+++ b/FullOverride/RunControl_fullOverride.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
   <si>
     <t>runname</t>
   </si>
@@ -185,6 +185,30 @@
   </si>
   <si>
     <t>RS1.ADC</t>
+  </si>
+  <si>
+    <t>RS2.Cap</t>
+  </si>
+  <si>
+    <t>RS3.Cap</t>
+  </si>
+  <si>
+    <t>RS4.Cap</t>
+  </si>
+  <si>
+    <t>RS5.Cap</t>
+  </si>
+  <si>
+    <t>RS2.ADC</t>
+  </si>
+  <si>
+    <t>RS3.ADC</t>
+  </si>
+  <si>
+    <t>RS4.ADC</t>
+  </si>
+  <si>
+    <t>RS5.ADC</t>
   </si>
 </sst>
 </file>
@@ -609,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AB19"/>
+  <dimension ref="A4:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,13 +1531,6 @@
       <c r="V18">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="W18">
-        <f t="shared" ref="W18:W19" si="2">0.0797</f>
-        <v>7.9699999999999993E-2</v>
-      </c>
-      <c r="X18">
-        <v>0.12</v>
-      </c>
       <c r="Y18">
         <v>20</v>
       </c>
@@ -1529,7 +1546,7 @@
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C19" t="b">
         <v>1</v>
@@ -1544,7 +1561,7 @@
         <v>6</v>
       </c>
       <c r="G19" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1586,18 +1603,11 @@
         <v>53</v>
       </c>
       <c r="U19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V19">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="W19">
-        <f t="shared" si="2"/>
-        <v>7.9699999999999993E-2</v>
-      </c>
-      <c r="X19">
-        <v>0.12</v>
-      </c>
       <c r="Y19">
         <v>20</v>
       </c>
@@ -1611,12 +1621,628 @@
         <v>15</v>
       </c>
     </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>2000</v>
+      </c>
+      <c r="E20">
+        <v>30</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J20">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>16</v>
+      </c>
+      <c r="O20">
+        <v>20</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>5</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="T20" t="s">
+        <v>53</v>
+      </c>
+      <c r="U20" t="s">
+        <v>45</v>
+      </c>
+      <c r="V20">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y20">
+        <v>20</v>
+      </c>
+      <c r="Z20">
+        <v>20</v>
+      </c>
+      <c r="AA20">
+        <v>30</v>
+      </c>
+      <c r="AB20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2000</v>
+      </c>
+      <c r="E21">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J21">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>16</v>
+      </c>
+      <c r="O21">
+        <v>20</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>5</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="T21" t="s">
+        <v>53</v>
+      </c>
+      <c r="U21" t="s">
+        <v>46</v>
+      </c>
+      <c r="V21">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y21">
+        <v>20</v>
+      </c>
+      <c r="Z21">
+        <v>20</v>
+      </c>
+      <c r="AA21">
+        <v>30</v>
+      </c>
+      <c r="AB21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>2000</v>
+      </c>
+      <c r="E22">
+        <v>30</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J22">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+      <c r="L22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" t="b">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22">
+        <v>20</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>5</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="T22" t="s">
+        <v>53</v>
+      </c>
+      <c r="U22" t="s">
+        <v>47</v>
+      </c>
+      <c r="V22">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y22">
+        <v>20</v>
+      </c>
+      <c r="Z22">
+        <v>20</v>
+      </c>
+      <c r="AA22">
+        <v>30</v>
+      </c>
+      <c r="AB22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>2000</v>
+      </c>
+      <c r="E24">
+        <v>30</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="L24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+      <c r="N24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O24">
+        <v>20</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>5</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24" t="s">
+        <v>53</v>
+      </c>
+      <c r="U24" t="s">
+        <v>43</v>
+      </c>
+      <c r="V24">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y24">
+        <v>20</v>
+      </c>
+      <c r="Z24">
+        <v>20</v>
+      </c>
+      <c r="AA24">
+        <v>30</v>
+      </c>
+      <c r="AB24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2000</v>
+      </c>
+      <c r="E25">
+        <v>30</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J25">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="L25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" t="b">
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25">
+        <v>20</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>5</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25" t="s">
+        <v>53</v>
+      </c>
+      <c r="U25" t="s">
+        <v>44</v>
+      </c>
+      <c r="V25">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y25">
+        <v>20</v>
+      </c>
+      <c r="Z25">
+        <v>20</v>
+      </c>
+      <c r="AA25">
+        <v>30</v>
+      </c>
+      <c r="AB25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>2000</v>
+      </c>
+      <c r="E26">
+        <v>30</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J26">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" t="b">
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26">
+        <v>20</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>5</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26" t="s">
+        <v>53</v>
+      </c>
+      <c r="U26" t="s">
+        <v>45</v>
+      </c>
+      <c r="V26">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y26">
+        <v>20</v>
+      </c>
+      <c r="Z26">
+        <v>20</v>
+      </c>
+      <c r="AA26">
+        <v>30</v>
+      </c>
+      <c r="AB26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>2000</v>
+      </c>
+      <c r="E27">
+        <v>30</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
+      <c r="N27" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27">
+        <v>20</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>5</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27" t="s">
+        <v>53</v>
+      </c>
+      <c r="U27" t="s">
+        <v>46</v>
+      </c>
+      <c r="V27">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y27">
+        <v>20</v>
+      </c>
+      <c r="Z27">
+        <v>20</v>
+      </c>
+      <c r="AA27">
+        <v>30</v>
+      </c>
+      <c r="AB27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>2000</v>
+      </c>
+      <c r="E28">
+        <v>30</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" t="b">
+        <v>1</v>
+      </c>
+      <c r="N28" t="s">
+        <v>16</v>
+      </c>
+      <c r="O28">
+        <v>20</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>5</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28" t="s">
+        <v>53</v>
+      </c>
+      <c r="U28" t="s">
+        <v>47</v>
+      </c>
+      <c r="V28">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y28">
+        <v>20</v>
+      </c>
+      <c r="Z28">
+        <v>20</v>
+      </c>
+      <c r="AA28">
+        <v>30</v>
+      </c>
+      <c r="AB28">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C28">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T28">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1630,7 +2256,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
graphs for UCRP report
</commit_message>
<xml_diff>
--- a/FullOverride/RunControl_fullOverride.xlsx
+++ b/FullOverride/RunControl_fullOverride.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
   <si>
     <t>runname</t>
   </si>
@@ -209,6 +209,21 @@
   </si>
   <si>
     <t>RS5.ADC</t>
+  </si>
+  <si>
+    <t>RS1.noCap</t>
+  </si>
+  <si>
+    <t>RS2.noCap</t>
+  </si>
+  <si>
+    <t>RS3.noCap</t>
+  </si>
+  <si>
+    <t>RS4.noCap</t>
+  </si>
+  <si>
+    <t>RS5.noCap</t>
   </si>
 </sst>
 </file>
@@ -633,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AB28"/>
+  <dimension ref="A4:AB34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +1869,7 @@
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C24" t="b">
         <v>1</v>
@@ -1931,7 +1946,7 @@
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C25" t="b">
         <v>1</v>
@@ -2008,7 +2023,7 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C26" t="b">
         <v>1</v>
@@ -2085,7 +2100,7 @@
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C27" t="b">
         <v>1</v>
@@ -2162,7 +2177,7 @@
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
@@ -2237,12 +2252,397 @@
         <v>15</v>
       </c>
     </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>2000</v>
+      </c>
+      <c r="E30">
+        <v>30</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J30">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N30" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30">
+        <v>20</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>5</v>
+      </c>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30" t="s">
+        <v>53</v>
+      </c>
+      <c r="U30" t="s">
+        <v>43</v>
+      </c>
+      <c r="V30">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y30">
+        <v>20</v>
+      </c>
+      <c r="Z30">
+        <v>20</v>
+      </c>
+      <c r="AA30">
+        <v>30</v>
+      </c>
+      <c r="AB30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>2000</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+      <c r="G31" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J31">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+      <c r="N31" t="s">
+        <v>16</v>
+      </c>
+      <c r="O31">
+        <v>20</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>5</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="T31" t="s">
+        <v>53</v>
+      </c>
+      <c r="U31" t="s">
+        <v>44</v>
+      </c>
+      <c r="V31">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y31">
+        <v>20</v>
+      </c>
+      <c r="Z31">
+        <v>20</v>
+      </c>
+      <c r="AA31">
+        <v>30</v>
+      </c>
+      <c r="AB31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>2000</v>
+      </c>
+      <c r="E32">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J32">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+      <c r="N32" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32">
+        <v>20</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>5</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32" t="s">
+        <v>53</v>
+      </c>
+      <c r="U32" t="s">
+        <v>45</v>
+      </c>
+      <c r="V32">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y32">
+        <v>20</v>
+      </c>
+      <c r="Z32">
+        <v>20</v>
+      </c>
+      <c r="AA32">
+        <v>30</v>
+      </c>
+      <c r="AB32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>2000</v>
+      </c>
+      <c r="E33">
+        <v>30</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J33">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+      <c r="N33" t="s">
+        <v>16</v>
+      </c>
+      <c r="O33">
+        <v>20</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <v>5</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="T33" t="s">
+        <v>53</v>
+      </c>
+      <c r="U33" t="s">
+        <v>46</v>
+      </c>
+      <c r="V33">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y33">
+        <v>20</v>
+      </c>
+      <c r="Z33">
+        <v>20</v>
+      </c>
+      <c r="AA33">
+        <v>30</v>
+      </c>
+      <c r="AB33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>2000</v>
+      </c>
+      <c r="E34">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+      <c r="G34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" t="b">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J34">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+      <c r="L34" t="b">
+        <v>1</v>
+      </c>
+      <c r="M34" t="b">
+        <v>0</v>
+      </c>
+      <c r="N34" t="s">
+        <v>16</v>
+      </c>
+      <c r="O34">
+        <v>20</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>5</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34" t="s">
+        <v>53</v>
+      </c>
+      <c r="U34" t="s">
+        <v>47</v>
+      </c>
+      <c r="V34">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="Y34">
+        <v>20</v>
+      </c>
+      <c r="Z34">
+        <v>20</v>
+      </c>
+      <c r="AA34">
+        <v>30</v>
+      </c>
+      <c r="AB34">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C28 C30:C34">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T5:T28 T30:T34">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2255,12 +2655,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2286,53 +2687,51 @@
         <v>43</v>
       </c>
       <c r="B2">
-        <v>0.05</v>
-      </c>
-      <c r="C2">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="C2" s="13">
         <v>0.1</v>
       </c>
       <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="E2" s="9">
         <f>B2-C2^2/2</f>
-        <v>4.4999999999999998E-2</v>
+        <v>7.2499999999999995E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C3">
+        <v>44</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="8">
         <v>0.1</v>
       </c>
       <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E17" si="0">B3-C3^2/2</f>
-        <v>6.5000000000000002E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <v>0.08</v>
-      </c>
-      <c r="C4">
+        <v>44</v>
+      </c>
+      <c r="B4" s="7">
+        <v>5.3749999999999999E-2</v>
+      </c>
+      <c r="C4" s="8">
         <v>0.1</v>
       </c>
       <c r="D4">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-2</v>
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
+        <v>5.3749999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2340,7 +2739,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="7">
-        <v>0.05</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="C5" s="8">
         <v>0.1</v>
@@ -2349,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="7">
-        <v>0.05</v>
+        <v>5.7500000000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2357,7 +2756,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="7">
-        <v>5.3749999999999999E-2</v>
+        <v>6.1249999999999999E-2</v>
       </c>
       <c r="C6" s="8">
         <v>0.1</v>
@@ -2366,7 +2765,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="7">
-        <v>5.3749999999999999E-2</v>
+        <v>6.1249999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,7 +2773,7 @@
         <v>44</v>
       </c>
       <c r="B7" s="7">
-        <v>5.7500000000000002E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="C7" s="8">
         <v>0.1</v>
@@ -2383,7 +2782,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="7">
-        <v>5.7500000000000002E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2391,7 +2790,7 @@
         <v>44</v>
       </c>
       <c r="B8" s="7">
-        <v>6.1249999999999999E-2</v>
+        <v>6.8750000000000006E-2</v>
       </c>
       <c r="C8" s="8">
         <v>0.1</v>
@@ -2400,7 +2799,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="7">
-        <v>6.1249999999999999E-2</v>
+        <v>6.8750000000000006E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,77 +2807,79 @@
         <v>44</v>
       </c>
       <c r="B9" s="7">
-        <v>6.5000000000000002E-2</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="C9" s="8">
         <v>0.1</v>
       </c>
       <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7">
-        <v>6.5000000000000002E-2</v>
+        <v>24</v>
+      </c>
+      <c r="E9" s="9">
+        <f>B9-C9^2/2</f>
+        <v>7.2499999999999995E-2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="7">
-        <v>6.8750000000000006E-2</v>
-      </c>
-      <c r="C10" s="8">
+        <v>45</v>
+      </c>
+      <c r="B10">
+        <v>0.05</v>
+      </c>
+      <c r="C10">
         <v>0.1</v>
       </c>
       <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="7">
-        <v>6.8750000000000006E-2</v>
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <f>B10-C10^2/2</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="7">
-        <v>7.7499999999999999E-2</v>
-      </c>
-      <c r="C11" s="8">
+        <v>45</v>
+      </c>
+      <c r="B11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C11">
         <v>0.1</v>
       </c>
       <c r="D11">
-        <v>24</v>
-      </c>
-      <c r="E11" s="9">
-        <f t="shared" si="0"/>
-        <v>7.2499999999999995E-2</v>
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <f>B11-C11^2/2</f>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="10">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C12" s="11">
+      <c r="B12">
+        <v>0.08</v>
+      </c>
+      <c r="C12">
         <v>0.1</v>
       </c>
       <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12" s="9">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <f>B12-C12^2/2</f>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="10">
-        <v>6.5000000000000002E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="C13" s="11">
         <v>0.1</v>
@@ -2487,80 +2888,80 @@
         <v>5</v>
       </c>
       <c r="E13" s="9">
+        <f t="shared" ref="E13:E17" si="0">B13-C13^2/2</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="10">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9">
         <f t="shared" si="0"/>
         <v>0.06</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="10">
-        <v>7.7499999999999999E-2</v>
-      </c>
-      <c r="C14" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-      <c r="E14" s="9">
-        <f t="shared" si="0"/>
-        <v>7.2499999999999995E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="12">
-        <v>0.06</v>
-      </c>
-      <c r="C15" s="13">
+      <c r="B15" s="10">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="C15" s="11">
         <v>0.1</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E15" s="9">
         <f t="shared" si="0"/>
-        <v>5.4999999999999993E-2</v>
+        <v>7.2499999999999995E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B16" s="12">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="C16" s="13">
         <v>0.1</v>
       </c>
       <c r="D16">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E16" s="9">
         <f t="shared" si="0"/>
-        <v>7.4999999999999997E-2</v>
+        <v>5.4999999999999993E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B17">
-        <v>7.7499999999999999E-2</v>
+      <c r="B17" s="12">
+        <v>0.08</v>
       </c>
       <c r="C17" s="13">
         <v>0.1</v>
       </c>
       <c r="D17">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E17" s="9">
         <f t="shared" si="0"/>
-        <v>7.2499999999999995E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>